<commit_message>
agrega tablas 0 y 50 cm
</commit_message>
<xml_diff>
--- a/Pruebas distancia.xlsx
+++ b/Pruebas distancia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="60" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="100" sheetId="5" r:id="rId5"/>
     <sheet name="110" sheetId="6" r:id="rId6"/>
     <sheet name="120" sheetId="7" r:id="rId7"/>
+    <sheet name="0" sheetId="8" r:id="rId8"/>
+    <sheet name="50" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="4">
   <si>
     <t>Grados</t>
   </si>
@@ -96,12 +98,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -120,15 +118,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -355,11 +349,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1999696560"/>
-        <c:axId val="-1962314832"/>
+        <c:axId val="348676544"/>
+        <c:axId val="348681248"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1999696560"/>
+        <c:axId val="348676544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962314832"/>
+        <c:crossAx val="348681248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +400,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962314832"/>
+        <c:axId val="348681248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +434,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1999696560"/>
+        <c:crossAx val="348676544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -674,11 +668,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1998036048"/>
-        <c:axId val="-1998032656"/>
+        <c:axId val="348710080"/>
+        <c:axId val="348713472"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1998036048"/>
+        <c:axId val="348710080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1998032656"/>
+        <c:crossAx val="348713472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -723,7 +717,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1998032656"/>
+        <c:axId val="348713472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -757,7 +751,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1998036048"/>
+        <c:crossAx val="348710080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1002,11 +996,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1962270160"/>
-        <c:axId val="-1962266128"/>
+        <c:axId val="309607552"/>
+        <c:axId val="309610400"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1962270160"/>
+        <c:axId val="309607552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1037,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962266128"/>
+        <c:crossAx val="309610400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1051,7 +1045,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962266128"/>
+        <c:axId val="309610400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962270160"/>
+        <c:crossAx val="309607552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1123,13 +1117,11 @@
               <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Mínima and Máxima</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1332,11 +1324,1277 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1962235440"/>
-        <c:axId val="-1962231408"/>
+        <c:axId val="348727424"/>
+        <c:axId val="348731456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1962235440"/>
+        <c:axId val="348727424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Grados</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348731456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348731456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348727424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Mínima and Máxima</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mínima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'100'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'100'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Máxima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'100'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'100'!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="348772784"/>
+        <c:axId val="348776816"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="348772784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Grados</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348776816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348776816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348772784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Mínima and Máxima</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'110'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mínima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'110'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'110'!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'110'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Máxima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'110'!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'110'!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="348810544"/>
+        <c:axId val="348814576"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="348810544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Grados</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348814576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="348814576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348810544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:t>Mínima/- and Máxima/-</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'120'!$A$1:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Grados</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'120'!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'120'!$A$1:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Grados</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'120'!$C$1:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>360.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351553840"/>
+        <c:axId val="351557872"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="351553840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Grados/26</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351557872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="351557872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351553840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mínima and Máxima</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'0'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mínima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'0'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'0'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'0'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Máxima</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="25400" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'0'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'0'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>330.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>360.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351590528"/>
+        <c:axId val="351594560"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="351590528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,7 +2633,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962231408"/>
+        <c:crossAx val="351594560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1383,7 +2641,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1962231408"/>
+        <c:axId val="351594560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +2675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962235440"/>
+        <c:crossAx val="351590528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1439,7 +2697,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1476,7 +2734,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100'!$B$1</c:f>
+              <c:f>'50'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1499,10 +2757,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'100'!$A$2:$A$9</c:f>
+              <c:f>'50'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>26.0</c:v>
                 </c:pt>
@@ -1520,45 +2778,33 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'100'!$B$2:$B$9</c:f>
+              <c:f>'50'!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>120.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>90.0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.0</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.0</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.0</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>180.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>240.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>330.0</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,7 +2815,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'100'!$C$1</c:f>
+              <c:f>'50'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1592,10 +2838,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'100'!$A$2:$A$9</c:f>
+              <c:f>'50'!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>26.0</c:v>
                 </c:pt>
@@ -1613,27 +2859,21 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'100'!$C$2:$C$9</c:f>
+              <c:f>'50'!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>180.0</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>330.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>330.0</c:v>
+                  <c:v>360.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>360.0</c:v>
@@ -1645,12 +2885,6 @@
                   <c:v>360.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>360.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>360.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>360.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1665,11 +2899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1996786224"/>
-        <c:axId val="-1996782192"/>
+        <c:axId val="309105392"/>
+        <c:axId val="309108784"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-1996786224"/>
+        <c:axId val="309105392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +2942,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1996782192"/>
+        <c:crossAx val="309108784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +2950,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1996782192"/>
+        <c:axId val="309108784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,661 +2984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1996786224"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="1600"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Mínima and Máxima</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'110'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mínima</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="3366CC">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="3366CC"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>'110'!$A$2:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-9.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'110'!$B$2:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>150.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>240.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>300.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'110'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Máxima</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DC3912">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="DC3912"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>'110'!$A$2:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>26.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-9.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'110'!$C$2:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>160.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>300.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>360.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>360.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>360.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>360.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-1996745408"/>
-        <c:axId val="-1996741376"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="-1996745408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Grados</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1996741376"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-1996741376"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1996745408"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="1"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr sz="1600"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Mínima/- and Máxima/-</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="3366CC">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="3366CC"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>'120'!$A$1:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Grados</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'120'!$B$1:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>150.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>120.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>180.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>240.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="DC3912">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="25400" cmpd="sng">
-              <a:solidFill>
-                <a:srgbClr val="DC3912"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>'120'!$A$1:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>Grados</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'120'!$C$1:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>300.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>330.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>360.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-1962201392"/>
-        <c:axId val="-1962197360"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="-1962201392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr lvl="0">
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Grados/26</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1962197360"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-1962197360"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="B7B7B7"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="47625">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr lvl="0">
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1962201392"/>
+        <c:crossAx val="309105392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2443,7 +3023,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2478,7 +3058,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2537,18 +3117,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2572,18 +3152,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2618,7 +3198,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2653,7 +3233,77 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3258,9 +3908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -3373,9 +4021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -3491,9 +4137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -3607,10 +4251,134 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
+        <v>210</v>
+      </c>
+      <c r="C3" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>120</v>
+      </c>
+      <c r="C5" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>90</v>
+      </c>
+      <c r="C6" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>120</v>
+      </c>
+      <c r="C7" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>180</v>
+      </c>
+      <c r="C8" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2">
+        <v>-9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>240</v>
+      </c>
+      <c r="C9" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <f>MAX(A1:C10)</f>
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3630,11 +4398,11 @@
       <c r="A2" s="2">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+      <c r="B2" s="2">
+        <v>150</v>
+      </c>
+      <c r="C2" s="2">
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3642,7 +4410,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C3" s="2">
         <v>330</v>
@@ -3653,10 +4421,10 @@
         <v>16</v>
       </c>
       <c r="B4" s="2">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="C4" s="2">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3664,7 +4432,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="C5" s="2">
         <v>330</v>
@@ -3675,49 +4443,134 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>90</v>
+        <v>300</v>
       </c>
       <c r="C6" s="2">
-        <v>330</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>120</v>
-      </c>
-      <c r="C7" s="2">
-        <v>330</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
-        <v>-4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>180</v>
-      </c>
-      <c r="C8" s="2">
-        <v>330</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2">
-        <v>-9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>240</v>
-      </c>
-      <c r="C9" s="2">
-        <v>360</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2">
+        <v>150</v>
+      </c>
+      <c r="C2" s="2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2">
+        <v>120</v>
+      </c>
+      <c r="C3" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>180</v>
+      </c>
+      <c r="C5" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>240</v>
+      </c>
+      <c r="C6" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>300</v>
+      </c>
+      <c r="C7" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>